<commit_message>
Lab 6 Checked In
WOOOOOOOOOOOOOOOOOOOOOOOOOOOOOOOOOOOOOOOOOOOOOOOOOOOOOOOOOOOOOOOOOOOOOOOOOOOOOOOOOOOOOOOOOO
</commit_message>
<xml_diff>
--- a/Lab 6/Data/Run_10.xlsx
+++ b/Lab 6/Data/Run_10.xlsx
@@ -1329,17 +1329,32 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="180038272"/>
-        <c:axId val="180040832"/>
+        <c:axId val="139198848"/>
+        <c:axId val="139200768"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="180038272"/>
+        <c:axId val="139198848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Time (ms)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
           <c:layout/>
           <c:overlay val="0"/>
         </c:title>
@@ -1347,12 +1362,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="180040832"/>
+        <c:crossAx val="139200768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="180040832"/>
+        <c:axId val="139200768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1360,6 +1375,21 @@
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Heading (degrees)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
           <c:layout/>
           <c:overlay val="0"/>
         </c:title>
@@ -1367,7 +1397,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="180038272"/>
+        <c:crossAx val="139198848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1708,8 +1738,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q12" sqref="Q12"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>